<commit_message>
começo do codigo c# e aliteraçẽos no excel
</commit_message>
<xml_diff>
--- a/Resource/Tarefas da Semana.xlsx
+++ b/Resource/Tarefas da Semana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\S.T.A.R\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF53D9-9FBC-40CD-B9B4-B70275B09708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71390F1B-7155-424F-982A-CB827BB6E17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeamento" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>DATA</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t xml:space="preserve">Implementação da API e suporte nas varias areas e </t>
   </si>
+  <si>
+    <t>Começo do UI do c#, Começo do Relatorio do Rosa</t>
+  </si>
 </sst>
 </file>
 
@@ -897,9 +900,39 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -909,12 +942,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -924,30 +951,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -957,6 +960,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -966,22 +987,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
@@ -991,24 +1012,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1293,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,37 +1309,37 @@
   <sheetData>
     <row r="1" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9 16383:16384" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="36"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="str">
+      <c r="B3" s="29" t="str">
         <f>TEXT(XFC3, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD3, "DD/MM/YYYY")</f>
         <v>03/02/2025 até 09/02/2025</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
       <c r="XFC3" s="2">
         <v>45691</v>
       </c>
@@ -1345,19 +1348,19 @@
       </c>
     </row>
     <row r="4" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="str">
+      <c r="B4" s="31" t="str">
         <f t="shared" ref="B4:B23" si="0">TEXT(XFC4, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD4, "DD/MM/YYYY")</f>
         <v>10/02/2025 até 16/02/2025</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="33"/>
       <c r="XFC4" s="2">
         <v>45698</v>
       </c>
@@ -1366,17 +1369,19 @@
       </c>
     </row>
     <row r="5" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="str">
+      <c r="B5" s="31" t="str">
         <f t="shared" si="0"/>
         <v>17/02/2025 até 23/02/2025</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="33"/>
       <c r="XFC5" s="2">
         <v>45705</v>
       </c>
@@ -1385,17 +1390,17 @@
       </c>
     </row>
     <row r="6" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="str">
+      <c r="B6" s="31" t="str">
         <f t="shared" si="0"/>
         <v>24/02/2025 até 02/03/2025</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="33"/>
       <c r="XFC6" s="2">
         <v>45712</v>
       </c>
@@ -1404,17 +1409,17 @@
       </c>
     </row>
     <row r="7" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="str">
+      <c r="B7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>03/03/2025 até 09/03/2025</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="33"/>
       <c r="XFC7" s="2">
         <v>45719</v>
       </c>
@@ -1423,17 +1428,17 @@
       </c>
     </row>
     <row r="8" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="str">
+      <c r="B8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>10/03/2025 até 16/03/2025</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="33"/>
       <c r="XFC8" s="2">
         <v>45726</v>
       </c>
@@ -1442,17 +1447,17 @@
       </c>
     </row>
     <row r="9" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="str">
+      <c r="B9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>17/03/2025 até 23/03/2025</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="33"/>
       <c r="XFC9" s="2">
         <v>45733</v>
       </c>
@@ -1461,17 +1466,17 @@
       </c>
     </row>
     <row r="10" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="str">
+      <c r="B10" s="31" t="str">
         <f t="shared" si="0"/>
         <v>24/03/2025 até 30/03/2025</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="33"/>
       <c r="XFC10" s="2">
         <v>45740</v>
       </c>
@@ -1480,17 +1485,17 @@
       </c>
     </row>
     <row r="11" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="str">
+      <c r="B11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>31/03/2025 até 06/04/2025</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="33"/>
       <c r="XFC11" s="2">
         <v>45747</v>
       </c>
@@ -1499,17 +1504,17 @@
       </c>
     </row>
     <row r="12" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="str">
+      <c r="B12" s="31" t="str">
         <f t="shared" si="0"/>
         <v>07/04/2025 até 13/04/2025</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="33"/>
       <c r="XFC12" s="2">
         <v>45754</v>
       </c>
@@ -1518,17 +1523,17 @@
       </c>
     </row>
     <row r="13" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="str">
+      <c r="B13" s="31" t="str">
         <f t="shared" si="0"/>
         <v>14/04/2025 até 20/04/2025</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="33"/>
       <c r="XFC13" s="2">
         <v>45761</v>
       </c>
@@ -1537,17 +1542,17 @@
       </c>
     </row>
     <row r="14" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="str">
+      <c r="B14" s="31" t="str">
         <f t="shared" si="0"/>
         <v>21/04/2025 até 27/04/2025</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="33"/>
       <c r="XFC14" s="2">
         <v>45768</v>
       </c>
@@ -1556,17 +1561,17 @@
       </c>
     </row>
     <row r="15" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="26" t="str">
+      <c r="B15" s="31" t="str">
         <f t="shared" si="0"/>
         <v>28/04/2025 até 04/05/2025</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="33"/>
       <c r="XFC15" s="2">
         <v>45775</v>
       </c>
@@ -1575,17 +1580,17 @@
       </c>
     </row>
     <row r="16" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="str">
+      <c r="B16" s="31" t="str">
         <f t="shared" si="0"/>
         <v>05/05/2025 até 11/05/2025</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="33"/>
       <c r="XFC16" s="2">
         <v>45782</v>
       </c>
@@ -1594,17 +1599,17 @@
       </c>
     </row>
     <row r="17" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="26" t="str">
+      <c r="B17" s="31" t="str">
         <f t="shared" si="0"/>
         <v>12/05/2025 até 18/05/2025</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="33"/>
       <c r="XFC17" s="2">
         <v>45789</v>
       </c>
@@ -1613,17 +1618,17 @@
       </c>
     </row>
     <row r="18" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="str">
+      <c r="B18" s="31" t="str">
         <f t="shared" si="0"/>
         <v>19/05/2025 até 25/05/2025</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="33"/>
       <c r="XFC18" s="2">
         <v>45796</v>
       </c>
@@ -1632,17 +1637,17 @@
       </c>
     </row>
     <row r="19" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="str">
+      <c r="B19" s="31" t="str">
         <f t="shared" si="0"/>
         <v>26/05/2025 até 01/06/2025</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="33"/>
       <c r="XFC19" s="2">
         <v>45803</v>
       </c>
@@ -1651,17 +1656,17 @@
       </c>
     </row>
     <row r="20" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="str">
+      <c r="B20" s="31" t="str">
         <f t="shared" si="0"/>
         <v>02/06/2025 até 08/06/2025</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="33"/>
       <c r="XFC20" s="2">
         <v>45810</v>
       </c>
@@ -1670,17 +1675,17 @@
       </c>
     </row>
     <row r="21" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="str">
+      <c r="B21" s="31" t="str">
         <f t="shared" si="0"/>
         <v>09/06/2025 até 15/06/2025</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="33"/>
       <c r="XFC21" s="2">
         <v>45817</v>
       </c>
@@ -1689,17 +1694,17 @@
       </c>
     </row>
     <row r="22" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="31" t="str">
         <f t="shared" si="0"/>
         <v>16/06/2025 até 22/06/2025</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="33"/>
       <c r="XFC22" s="2">
         <v>45824</v>
       </c>
@@ -1708,17 +1713,17 @@
       </c>
     </row>
     <row r="23" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="str">
+      <c r="B23" s="31" t="str">
         <f t="shared" si="0"/>
         <v>23/06/2025 até 29/06/2025</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="33"/>
       <c r="XFC23" s="2">
         <v>45831</v>
       </c>
@@ -1727,17 +1732,17 @@
       </c>
     </row>
     <row r="24" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="str">
+      <c r="B24" s="31" t="str">
         <f t="shared" ref="B24:B25" si="1">TEXT(XFC24, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD24, "DD/MM/YYYY")</f>
         <v>30/06/2025 até 06/07/2025</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="33"/>
       <c r="XFC24" s="2">
         <v>45838</v>
       </c>
@@ -1746,17 +1751,17 @@
       </c>
     </row>
     <row r="25" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="str">
+      <c r="B25" s="36" t="str">
         <f t="shared" si="1"/>
         <v>07/07/2025 até 13/07/2025</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="30"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="38"/>
       <c r="XFC25" s="2">
         <v>45845</v>
       </c>
@@ -1765,40 +1770,70 @@
       </c>
     </row>
     <row r="26" spans="2:9 16383:16384" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
     </row>
     <row r="27" spans="2:9 16383:16384" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B16:C16"/>
@@ -1815,61 +1850,31 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1911,16 +1916,16 @@
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="47"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1941,16 +1946,16 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
       <c r="L8" s="13" t="s">
         <v>13</v>
       </c>
@@ -4161,14 +4166,14 @@
     <row r="153" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="20"/>
       <c r="C153" s="18"/>
-      <c r="D153" s="42"/>
-      <c r="E153" s="43"/>
-      <c r="F153" s="43"/>
-      <c r="G153" s="43"/>
-      <c r="H153" s="43"/>
-      <c r="I153" s="43"/>
-      <c r="J153" s="43"/>
-      <c r="K153" s="44"/>
+      <c r="D153" s="48"/>
+      <c r="E153" s="49"/>
+      <c r="F153" s="49"/>
+      <c r="G153" s="49"/>
+      <c r="H153" s="49"/>
+      <c r="I153" s="49"/>
+      <c r="J153" s="49"/>
+      <c r="K153" s="50"/>
       <c r="L153" s="18"/>
       <c r="M153" s="6"/>
       <c r="N153" s="19"/>
@@ -4177,6 +4182,135 @@
   </sheetData>
   <autoFilter ref="C7" xr:uid="{6C0B39F1-AC0F-4876-8C89-BECC8B704A99}"/>
   <mergeCells count="147">
+    <mergeCell ref="D152:K152"/>
+    <mergeCell ref="D153:K153"/>
+    <mergeCell ref="D147:K147"/>
+    <mergeCell ref="D148:K148"/>
+    <mergeCell ref="D149:K149"/>
+    <mergeCell ref="D150:K150"/>
+    <mergeCell ref="D151:K151"/>
+    <mergeCell ref="D142:K142"/>
+    <mergeCell ref="D143:K143"/>
+    <mergeCell ref="D144:K144"/>
+    <mergeCell ref="D145:K145"/>
+    <mergeCell ref="D146:K146"/>
+    <mergeCell ref="D137:K137"/>
+    <mergeCell ref="D138:K138"/>
+    <mergeCell ref="D139:K139"/>
+    <mergeCell ref="D140:K140"/>
+    <mergeCell ref="D141:K141"/>
+    <mergeCell ref="D132:K132"/>
+    <mergeCell ref="D133:K133"/>
+    <mergeCell ref="D134:K134"/>
+    <mergeCell ref="D135:K135"/>
+    <mergeCell ref="D136:K136"/>
+    <mergeCell ref="D127:K127"/>
+    <mergeCell ref="D128:K128"/>
+    <mergeCell ref="D129:K129"/>
+    <mergeCell ref="D130:K130"/>
+    <mergeCell ref="D131:K131"/>
+    <mergeCell ref="D122:K122"/>
+    <mergeCell ref="D123:K123"/>
+    <mergeCell ref="D124:K124"/>
+    <mergeCell ref="D125:K125"/>
+    <mergeCell ref="D126:K126"/>
+    <mergeCell ref="D117:K117"/>
+    <mergeCell ref="D118:K118"/>
+    <mergeCell ref="D119:K119"/>
+    <mergeCell ref="D120:K120"/>
+    <mergeCell ref="D121:K121"/>
+    <mergeCell ref="D112:K112"/>
+    <mergeCell ref="D113:K113"/>
+    <mergeCell ref="D114:K114"/>
+    <mergeCell ref="D115:K115"/>
+    <mergeCell ref="D116:K116"/>
+    <mergeCell ref="D107:K107"/>
+    <mergeCell ref="D108:K108"/>
+    <mergeCell ref="D109:K109"/>
+    <mergeCell ref="D110:K110"/>
+    <mergeCell ref="D111:K111"/>
+    <mergeCell ref="D102:K102"/>
+    <mergeCell ref="D103:K103"/>
+    <mergeCell ref="D104:K104"/>
+    <mergeCell ref="D105:K105"/>
+    <mergeCell ref="D106:K106"/>
+    <mergeCell ref="D97:K97"/>
+    <mergeCell ref="D98:K98"/>
+    <mergeCell ref="D99:K99"/>
+    <mergeCell ref="D100:K100"/>
+    <mergeCell ref="D101:K101"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D87:K87"/>
+    <mergeCell ref="D88:K88"/>
+    <mergeCell ref="D89:K89"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D82:K82"/>
+    <mergeCell ref="D83:K83"/>
+    <mergeCell ref="D84:K84"/>
+    <mergeCell ref="D85:K85"/>
+    <mergeCell ref="D86:K86"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D72:K72"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="D74:K74"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="D68:K68"/>
+    <mergeCell ref="D69:K69"/>
+    <mergeCell ref="D70:K70"/>
+    <mergeCell ref="D71:K71"/>
+    <mergeCell ref="D62:K62"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:K64"/>
+    <mergeCell ref="D65:K65"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D57:K57"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:K59"/>
+    <mergeCell ref="D60:K60"/>
+    <mergeCell ref="D61:K61"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="D54:K54"/>
+    <mergeCell ref="D55:K55"/>
+    <mergeCell ref="D56:K56"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="D48:K48"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="D45:K45"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="D31:K31"/>
+    <mergeCell ref="D32:K32"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="D34:K34"/>
+    <mergeCell ref="D35:K35"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
@@ -4195,135 +4329,6 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D23:K23"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="D32:K32"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="D35:K35"/>
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="D48:K48"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="D43:K43"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="D57:K57"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:K59"/>
-    <mergeCell ref="D60:K60"/>
-    <mergeCell ref="D61:K61"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="D54:K54"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="D67:K67"/>
-    <mergeCell ref="D68:K68"/>
-    <mergeCell ref="D69:K69"/>
-    <mergeCell ref="D70:K70"/>
-    <mergeCell ref="D71:K71"/>
-    <mergeCell ref="D62:K62"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:K64"/>
-    <mergeCell ref="D65:K65"/>
-    <mergeCell ref="D66:K66"/>
-    <mergeCell ref="D77:K77"/>
-    <mergeCell ref="D78:K78"/>
-    <mergeCell ref="D79:K79"/>
-    <mergeCell ref="D80:K80"/>
-    <mergeCell ref="D81:K81"/>
-    <mergeCell ref="D72:K72"/>
-    <mergeCell ref="D73:K73"/>
-    <mergeCell ref="D74:K74"/>
-    <mergeCell ref="D75:K75"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D87:K87"/>
-    <mergeCell ref="D88:K88"/>
-    <mergeCell ref="D89:K89"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D82:K82"/>
-    <mergeCell ref="D83:K83"/>
-    <mergeCell ref="D84:K84"/>
-    <mergeCell ref="D85:K85"/>
-    <mergeCell ref="D86:K86"/>
-    <mergeCell ref="D97:K97"/>
-    <mergeCell ref="D98:K98"/>
-    <mergeCell ref="D99:K99"/>
-    <mergeCell ref="D100:K100"/>
-    <mergeCell ref="D101:K101"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D107:K107"/>
-    <mergeCell ref="D108:K108"/>
-    <mergeCell ref="D109:K109"/>
-    <mergeCell ref="D110:K110"/>
-    <mergeCell ref="D111:K111"/>
-    <mergeCell ref="D102:K102"/>
-    <mergeCell ref="D103:K103"/>
-    <mergeCell ref="D104:K104"/>
-    <mergeCell ref="D105:K105"/>
-    <mergeCell ref="D106:K106"/>
-    <mergeCell ref="D117:K117"/>
-    <mergeCell ref="D118:K118"/>
-    <mergeCell ref="D119:K119"/>
-    <mergeCell ref="D120:K120"/>
-    <mergeCell ref="D121:K121"/>
-    <mergeCell ref="D112:K112"/>
-    <mergeCell ref="D113:K113"/>
-    <mergeCell ref="D114:K114"/>
-    <mergeCell ref="D115:K115"/>
-    <mergeCell ref="D116:K116"/>
-    <mergeCell ref="D127:K127"/>
-    <mergeCell ref="D128:K128"/>
-    <mergeCell ref="D129:K129"/>
-    <mergeCell ref="D130:K130"/>
-    <mergeCell ref="D131:K131"/>
-    <mergeCell ref="D122:K122"/>
-    <mergeCell ref="D123:K123"/>
-    <mergeCell ref="D124:K124"/>
-    <mergeCell ref="D125:K125"/>
-    <mergeCell ref="D126:K126"/>
-    <mergeCell ref="D137:K137"/>
-    <mergeCell ref="D138:K138"/>
-    <mergeCell ref="D139:K139"/>
-    <mergeCell ref="D140:K140"/>
-    <mergeCell ref="D141:K141"/>
-    <mergeCell ref="D132:K132"/>
-    <mergeCell ref="D133:K133"/>
-    <mergeCell ref="D134:K134"/>
-    <mergeCell ref="D135:K135"/>
-    <mergeCell ref="D136:K136"/>
-    <mergeCell ref="D152:K152"/>
-    <mergeCell ref="D153:K153"/>
-    <mergeCell ref="D147:K147"/>
-    <mergeCell ref="D148:K148"/>
-    <mergeCell ref="D149:K149"/>
-    <mergeCell ref="D150:K150"/>
-    <mergeCell ref="D151:K151"/>
-    <mergeCell ref="D142:K142"/>
-    <mergeCell ref="D143:K143"/>
-    <mergeCell ref="D144:K144"/>
-    <mergeCell ref="D145:K145"/>
-    <mergeCell ref="D146:K146"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C153" xr:uid="{1F00872D-AE43-4317-8957-7AD9F526CA78}">
@@ -4339,7 +4344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FFB9743-59E5-4A0D-AEA9-FBA84F8DCEFF}">
   <dimension ref="B1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -4347,162 +4352,162 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="59"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="53"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="51"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52" t="s">
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52" t="s">
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="59"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="59"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="53"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="59"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="53"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="59"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="54" t="s">
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="56"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="53"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:K3"/>
+    <mergeCell ref="L2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="L4:O5"/>
     <mergeCell ref="D8:O9"/>
     <mergeCell ref="B8:C9"/>
     <mergeCell ref="D4:G5"/>
     <mergeCell ref="D6:G7"/>
     <mergeCell ref="H4:K5"/>
     <mergeCell ref="H6:K7"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:K3"/>
-    <mergeCell ref="L2:O3"/>
-    <mergeCell ref="B4:C5"/>
     <mergeCell ref="B6:C7"/>
-    <mergeCell ref="L4:O5"/>
     <mergeCell ref="L6:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
atualizacao de frontend, tarefas semanais e comunicacao
</commit_message>
<xml_diff>
--- a/Resource/Tarefas da Semana.xlsx
+++ b/Resource/Tarefas da Semana.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\S.T.A.R\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C1DF68-39C1-4F6A-84A0-252A753C8CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FE68EB-E5EA-42AA-9DEF-89FA93F2B0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planeamento" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>DATA</t>
   </si>
@@ -127,6 +127,27 @@
   <si>
     <t>Pesquisa/estudo sobre a parte de arduino</t>
   </si>
+  <si>
+    <t>Estudo do TPCClient</t>
+  </si>
+  <si>
+    <t>Tentativa do convivio com os designers e reunião de equipa para unir projetos</t>
+  </si>
+  <si>
+    <t>Apresentações do projeto</t>
+  </si>
+  <si>
+    <t>Tech4Good</t>
+  </si>
+  <si>
+    <t>Reunião de equipa com designers sem sucesso</t>
+  </si>
+  <si>
+    <t>Adaptação do codigo para MQTT e soldagem do material</t>
+  </si>
+  <si>
+    <t>Continuação da adição de novas features no projeto, começo do Protobuf, compra de material para o veiculo</t>
+  </si>
 </sst>
 </file>
 
@@ -918,18 +939,42 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,30 +987,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,6 +996,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -993,14 +1023,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1018,15 +1048,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1312,49 +1333,49 @@
   <dimension ref="A1:XFD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:I6"/>
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="15.73046875" customWidth="1"/>
-    <col min="4" max="9" width="25.73046875" customWidth="1"/>
-    <col min="16383" max="16384" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="9" width="25.7109375" customWidth="1"/>
+    <col min="16383" max="16384" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9 16383:16384" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:9 16383:16384" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9 16383:16384" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="2:9 16383:16384" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="29" t="str">
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="str">
         <f>TEXT(XFC3, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD3, "DD/MM/YYYY")</f>
         <v>03/02/2025 até 09/02/2025</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
       <c r="XFC3" s="2">
         <v>45691</v>
       </c>
@@ -1362,24 +1383,24 @@
         <v>45697</v>
       </c>
     </row>
-    <row r="4" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="30" t="str">
+    <row r="4" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="str">
         <f t="shared" ref="B4:B23" si="0">TEXT(XFC4, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD4, "DD/MM/YYYY")</f>
         <v>10/02/2025 até 16/02/2025</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="32"/>
+      <c r="I4" s="23"/>
       <c r="XFC4" s="2">
         <v>45698</v>
       </c>
@@ -1387,24 +1408,24 @@
         <v>45704</v>
       </c>
     </row>
-    <row r="5" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="30" t="str">
+    <row r="5" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="str">
         <f t="shared" si="0"/>
         <v>17/02/2025 até 23/02/2025</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="23"/>
       <c r="XFC5" s="2">
         <v>45705</v>
       </c>
@@ -1412,24 +1433,24 @@
         <v>45711</v>
       </c>
     </row>
-    <row r="6" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="30" t="str">
+    <row r="6" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="str">
         <f t="shared" si="0"/>
         <v>24/02/2025 até 02/03/2025</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="24" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="23"/>
       <c r="XFC6" s="2">
         <v>45712</v>
       </c>
@@ -1437,18 +1458,20 @@
         <v>45718</v>
       </c>
     </row>
-    <row r="7" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="30" t="str">
+    <row r="7" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="26" t="str">
         <f t="shared" si="0"/>
         <v>03/03/2025 até 09/03/2025</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="32"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
       <c r="XFC7" s="2">
         <v>45719</v>
       </c>
@@ -1456,18 +1479,20 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="8" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="30" t="str">
+    <row r="8" spans="2:9 16383:16384" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="str">
         <f t="shared" si="0"/>
         <v>10/03/2025 até 16/03/2025</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="32"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
       <c r="XFC8" s="2">
         <v>45726</v>
       </c>
@@ -1475,18 +1500,20 @@
         <v>45732</v>
       </c>
     </row>
-    <row r="9" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="30" t="str">
+    <row r="9" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="str">
         <f t="shared" si="0"/>
         <v>17/03/2025 até 23/03/2025</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="32"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
       <c r="XFC9" s="2">
         <v>45733</v>
       </c>
@@ -1494,18 +1521,20 @@
         <v>45739</v>
       </c>
     </row>
-    <row r="10" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="30" t="str">
+    <row r="10" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="26" t="str">
         <f t="shared" si="0"/>
         <v>24/03/2025 até 30/03/2025</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="32"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
       <c r="XFC10" s="2">
         <v>45740</v>
       </c>
@@ -1513,18 +1542,20 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="11" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="30" t="str">
+    <row r="11" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="str">
         <f t="shared" si="0"/>
         <v>31/03/2025 até 06/04/2025</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="32"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
       <c r="XFC11" s="2">
         <v>45747</v>
       </c>
@@ -1532,18 +1563,20 @@
         <v>45753</v>
       </c>
     </row>
-    <row r="12" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="30" t="str">
+    <row r="12" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>07/04/2025 até 13/04/2025</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="32"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
       <c r="XFC12" s="2">
         <v>45754</v>
       </c>
@@ -1551,18 +1584,20 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="13" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="30" t="str">
+    <row r="13" spans="2:9 16383:16384" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>14/04/2025 até 20/04/2025</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="32"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
       <c r="XFC13" s="2">
         <v>45761</v>
       </c>
@@ -1570,18 +1605,18 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="14" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="30" t="str">
+    <row r="14" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>21/04/2025 até 27/04/2025</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="32"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
       <c r="XFC14" s="2">
         <v>45768</v>
       </c>
@@ -1589,18 +1624,18 @@
         <v>45774</v>
       </c>
     </row>
-    <row r="15" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="30" t="str">
+    <row r="15" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="str">
         <f t="shared" si="0"/>
         <v>28/04/2025 até 04/05/2025</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="32"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
       <c r="XFC15" s="2">
         <v>45775</v>
       </c>
@@ -1608,18 +1643,18 @@
         <v>45781</v>
       </c>
     </row>
-    <row r="16" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="30" t="str">
+    <row r="16" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>05/05/2025 até 11/05/2025</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="32"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
       <c r="XFC16" s="2">
         <v>45782</v>
       </c>
@@ -1627,18 +1662,18 @@
         <v>45788</v>
       </c>
     </row>
-    <row r="17" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="30" t="str">
+    <row r="17" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="str">
         <f t="shared" si="0"/>
         <v>12/05/2025 até 18/05/2025</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="32"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
       <c r="XFC17" s="2">
         <v>45789</v>
       </c>
@@ -1646,18 +1681,18 @@
         <v>45795</v>
       </c>
     </row>
-    <row r="18" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="30" t="str">
+    <row r="18" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="26" t="str">
         <f t="shared" si="0"/>
         <v>19/05/2025 até 25/05/2025</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="32"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
       <c r="XFC18" s="2">
         <v>45796</v>
       </c>
@@ -1665,18 +1700,18 @@
         <v>45802</v>
       </c>
     </row>
-    <row r="19" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="30" t="str">
+    <row r="19" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="26" t="str">
         <f t="shared" si="0"/>
         <v>26/05/2025 até 01/06/2025</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="32"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
       <c r="XFC19" s="2">
         <v>45803</v>
       </c>
@@ -1684,18 +1719,18 @@
         <v>45809</v>
       </c>
     </row>
-    <row r="20" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="30" t="str">
+    <row r="20" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="26" t="str">
         <f t="shared" si="0"/>
         <v>02/06/2025 até 08/06/2025</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="32"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
       <c r="XFC20" s="2">
         <v>45810</v>
       </c>
@@ -1703,18 +1738,18 @@
         <v>45816</v>
       </c>
     </row>
-    <row r="21" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="30" t="str">
+    <row r="21" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="26" t="str">
         <f t="shared" si="0"/>
         <v>09/06/2025 até 15/06/2025</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="32"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
       <c r="XFC21" s="2">
         <v>45817</v>
       </c>
@@ -1722,18 +1757,18 @@
         <v>45823</v>
       </c>
     </row>
-    <row r="22" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="30" t="str">
+    <row r="22" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="str">
         <f t="shared" si="0"/>
         <v>16/06/2025 até 22/06/2025</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="32"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
       <c r="XFC22" s="2">
         <v>45824</v>
       </c>
@@ -1741,18 +1776,18 @@
         <v>45830</v>
       </c>
     </row>
-    <row r="23" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="30" t="str">
+    <row r="23" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="26" t="str">
         <f t="shared" si="0"/>
         <v>23/06/2025 até 29/06/2025</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="32"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
       <c r="XFC23" s="2">
         <v>45831</v>
       </c>
@@ -1760,18 +1795,18 @@
         <v>45837</v>
       </c>
     </row>
-    <row r="24" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="30" t="str">
+    <row r="24" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="str">
         <f t="shared" ref="B24:B25" si="1">TEXT(XFC24, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD24, "DD/MM/YYYY")</f>
         <v>30/06/2025 até 06/07/2025</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="32"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
       <c r="XFC24" s="2">
         <v>45838</v>
       </c>
@@ -1779,18 +1814,18 @@
         <v>45844</v>
       </c>
     </row>
-    <row r="25" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="35" t="str">
+    <row r="25" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="28" t="str">
         <f t="shared" si="1"/>
         <v>07/07/2025 até 13/07/2025</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="37"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="30"/>
       <c r="XFC25" s="2">
         <v>45845</v>
       </c>
@@ -1798,16 +1833,96 @@
         <v>45851</v>
       </c>
     </row>
-    <row r="26" spans="2:9 16383:16384" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-    </row>
-    <row r="27" spans="2:9 16383:16384" x14ac:dyDescent="0.45">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+    <row r="26" spans="2:9 16383:16384" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+    </row>
+    <row r="27" spans="2:9 16383:16384" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B27:C27"/>
@@ -1824,86 +1939,6 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1918,43 +1953,43 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.73046875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" style="1" customWidth="1"/>
-    <col min="4" max="11" width="9.1328125" style="1"/>
-    <col min="12" max="13" width="19.265625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1328125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="9.140625" style="1"/>
+    <col min="12" max="13" width="19.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="2:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="2:22" ht="9" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:22" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:22" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
       <c r="L7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1968,23 +2003,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:22" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>45702</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="13" t="s">
         <v>13</v>
       </c>
@@ -1998,7 +2033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>45703</v>
       </c>
@@ -2024,7 +2059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>45703</v>
       </c>
@@ -2054,7 +2089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>45703</v>
       </c>
@@ -2077,7 +2112,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="38"/>
@@ -2092,7 +2127,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="38"/>
@@ -2107,7 +2142,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="38"/>
@@ -2122,7 +2157,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="17"/>
     </row>
-    <row r="15" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="38"/>
@@ -2137,7 +2172,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="17"/>
     </row>
-    <row r="16" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="38"/>
@@ -2152,7 +2187,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="17"/>
     </row>
-    <row r="17" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="38"/>
@@ -2167,7 +2202,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="17"/>
     </row>
-    <row r="18" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="38"/>
@@ -2182,7 +2217,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="17"/>
     </row>
-    <row r="19" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="38"/>
@@ -2197,7 +2232,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="17"/>
     </row>
-    <row r="20" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="38"/>
@@ -2212,7 +2247,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="38"/>
@@ -2227,7 +2262,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="38"/>
@@ -2242,7 +2277,7 @@
       <c r="M22" s="5"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="38"/>
@@ -2257,7 +2292,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="17"/>
     </row>
-    <row r="24" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="38"/>
@@ -2272,7 +2307,7 @@
       <c r="M24" s="5"/>
       <c r="N24" s="17"/>
     </row>
-    <row r="25" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="38"/>
@@ -2287,7 +2322,7 @@
       <c r="M25" s="5"/>
       <c r="N25" s="17"/>
     </row>
-    <row r="26" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="38"/>
@@ -2302,7 +2337,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="17"/>
     </row>
-    <row r="27" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="38"/>
@@ -2317,7 +2352,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="17"/>
     </row>
-    <row r="28" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="38"/>
@@ -2332,7 +2367,7 @@
       <c r="M28" s="5"/>
       <c r="N28" s="17"/>
     </row>
-    <row r="29" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="38"/>
@@ -2347,7 +2382,7 @@
       <c r="M29" s="5"/>
       <c r="N29" s="17"/>
     </row>
-    <row r="30" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="38"/>
@@ -2362,7 +2397,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="17"/>
     </row>
-    <row r="31" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="38"/>
@@ -2377,7 +2412,7 @@
       <c r="M31" s="5"/>
       <c r="N31" s="17"/>
     </row>
-    <row r="32" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="38"/>
@@ -2392,7 +2427,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="17"/>
     </row>
-    <row r="33" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="38"/>
@@ -2407,7 +2442,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="17"/>
     </row>
-    <row r="34" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="38"/>
@@ -2422,7 +2457,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="17"/>
     </row>
-    <row r="35" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="38"/>
@@ -2437,7 +2472,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="17"/>
     </row>
-    <row r="36" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="38"/>
@@ -2452,7 +2487,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="38"/>
@@ -2467,7 +2502,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="38"/>
@@ -2482,7 +2517,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="17"/>
     </row>
-    <row r="39" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="38"/>
@@ -2497,7 +2532,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="38"/>
@@ -2512,7 +2547,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="38"/>
@@ -2527,7 +2562,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="17"/>
     </row>
-    <row r="42" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="38"/>
@@ -2542,7 +2577,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="38"/>
@@ -2557,7 +2592,7 @@
       <c r="M43" s="5"/>
       <c r="N43" s="17"/>
     </row>
-    <row r="44" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="38"/>
@@ -2572,7 +2607,7 @@
       <c r="M44" s="5"/>
       <c r="N44" s="17"/>
     </row>
-    <row r="45" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="38"/>
@@ -2587,7 +2622,7 @@
       <c r="M45" s="5"/>
       <c r="N45" s="17"/>
     </row>
-    <row r="46" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="38"/>
@@ -2602,7 +2637,7 @@
       <c r="M46" s="5"/>
       <c r="N46" s="17"/>
     </row>
-    <row r="47" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="38"/>
@@ -2617,7 +2652,7 @@
       <c r="M47" s="5"/>
       <c r="N47" s="17"/>
     </row>
-    <row r="48" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="38"/>
@@ -2632,7 +2667,7 @@
       <c r="M48" s="5"/>
       <c r="N48" s="17"/>
     </row>
-    <row r="49" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="38"/>
@@ -2647,7 +2682,7 @@
       <c r="M49" s="5"/>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="38"/>
@@ -2662,7 +2697,7 @@
       <c r="M50" s="5"/>
       <c r="N50" s="17"/>
     </row>
-    <row r="51" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="38"/>
@@ -2677,7 +2712,7 @@
       <c r="M51" s="5"/>
       <c r="N51" s="17"/>
     </row>
-    <row r="52" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="38"/>
@@ -2692,7 +2727,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="17"/>
     </row>
-    <row r="53" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="38"/>
@@ -2707,7 +2742,7 @@
       <c r="M53" s="5"/>
       <c r="N53" s="17"/>
     </row>
-    <row r="54" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="38"/>
@@ -2722,7 +2757,7 @@
       <c r="M54" s="5"/>
       <c r="N54" s="17"/>
     </row>
-    <row r="55" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="38"/>
@@ -2737,7 +2772,7 @@
       <c r="M55" s="5"/>
       <c r="N55" s="17"/>
     </row>
-    <row r="56" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="38"/>
@@ -2752,7 +2787,7 @@
       <c r="M56" s="5"/>
       <c r="N56" s="17"/>
     </row>
-    <row r="57" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="38"/>
@@ -2767,7 +2802,7 @@
       <c r="M57" s="5"/>
       <c r="N57" s="17"/>
     </row>
-    <row r="58" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="38"/>
@@ -2782,7 +2817,7 @@
       <c r="M58" s="5"/>
       <c r="N58" s="17"/>
     </row>
-    <row r="59" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="38"/>
@@ -2797,7 +2832,7 @@
       <c r="M59" s="5"/>
       <c r="N59" s="17"/>
     </row>
-    <row r="60" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="38"/>
@@ -2812,7 +2847,7 @@
       <c r="M60" s="5"/>
       <c r="N60" s="17"/>
     </row>
-    <row r="61" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="38"/>
@@ -2827,7 +2862,7 @@
       <c r="M61" s="5"/>
       <c r="N61" s="17"/>
     </row>
-    <row r="62" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="38"/>
@@ -2842,7 +2877,7 @@
       <c r="M62" s="5"/>
       <c r="N62" s="17"/>
     </row>
-    <row r="63" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="38"/>
@@ -2857,7 +2892,7 @@
       <c r="M63" s="5"/>
       <c r="N63" s="17"/>
     </row>
-    <row r="64" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="38"/>
@@ -2872,7 +2907,7 @@
       <c r="M64" s="5"/>
       <c r="N64" s="17"/>
     </row>
-    <row r="65" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="38"/>
@@ -2887,7 +2922,7 @@
       <c r="M65" s="5"/>
       <c r="N65" s="17"/>
     </row>
-    <row r="66" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="38"/>
@@ -2902,7 +2937,7 @@
       <c r="M66" s="5"/>
       <c r="N66" s="17"/>
     </row>
-    <row r="67" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="38"/>
@@ -2917,7 +2952,7 @@
       <c r="M67" s="5"/>
       <c r="N67" s="17"/>
     </row>
-    <row r="68" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="38"/>
@@ -2932,7 +2967,7 @@
       <c r="M68" s="5"/>
       <c r="N68" s="17"/>
     </row>
-    <row r="69" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="38"/>
@@ -2947,7 +2982,7 @@
       <c r="M69" s="5"/>
       <c r="N69" s="17"/>
     </row>
-    <row r="70" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="38"/>
@@ -2962,7 +2997,7 @@
       <c r="M70" s="5"/>
       <c r="N70" s="17"/>
     </row>
-    <row r="71" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="38"/>
@@ -2977,7 +3012,7 @@
       <c r="M71" s="5"/>
       <c r="N71" s="17"/>
     </row>
-    <row r="72" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="38"/>
@@ -2992,7 +3027,7 @@
       <c r="M72" s="5"/>
       <c r="N72" s="17"/>
     </row>
-    <row r="73" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="38"/>
@@ -3007,7 +3042,7 @@
       <c r="M73" s="5"/>
       <c r="N73" s="17"/>
     </row>
-    <row r="74" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="38"/>
@@ -3022,7 +3057,7 @@
       <c r="M74" s="5"/>
       <c r="N74" s="17"/>
     </row>
-    <row r="75" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="38"/>
@@ -3037,7 +3072,7 @@
       <c r="M75" s="5"/>
       <c r="N75" s="17"/>
     </row>
-    <row r="76" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="38"/>
@@ -3052,7 +3087,7 @@
       <c r="M76" s="5"/>
       <c r="N76" s="17"/>
     </row>
-    <row r="77" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="38"/>
@@ -3067,7 +3102,7 @@
       <c r="M77" s="5"/>
       <c r="N77" s="17"/>
     </row>
-    <row r="78" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="38"/>
@@ -3082,7 +3117,7 @@
       <c r="M78" s="5"/>
       <c r="N78" s="17"/>
     </row>
-    <row r="79" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="38"/>
@@ -3097,7 +3132,7 @@
       <c r="M79" s="5"/>
       <c r="N79" s="17"/>
     </row>
-    <row r="80" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="38"/>
@@ -3112,7 +3147,7 @@
       <c r="M80" s="5"/>
       <c r="N80" s="17"/>
     </row>
-    <row r="81" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="38"/>
@@ -3127,7 +3162,7 @@
       <c r="M81" s="5"/>
       <c r="N81" s="17"/>
     </row>
-    <row r="82" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="38"/>
@@ -3142,7 +3177,7 @@
       <c r="M82" s="5"/>
       <c r="N82" s="17"/>
     </row>
-    <row r="83" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="38"/>
@@ -3157,7 +3192,7 @@
       <c r="M83" s="5"/>
       <c r="N83" s="17"/>
     </row>
-    <row r="84" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="38"/>
@@ -3172,7 +3207,7 @@
       <c r="M84" s="5"/>
       <c r="N84" s="17"/>
     </row>
-    <row r="85" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="38"/>
@@ -3187,7 +3222,7 @@
       <c r="M85" s="5"/>
       <c r="N85" s="17"/>
     </row>
-    <row r="86" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="38"/>
@@ -3202,7 +3237,7 @@
       <c r="M86" s="5"/>
       <c r="N86" s="17"/>
     </row>
-    <row r="87" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="38"/>
@@ -3217,7 +3252,7 @@
       <c r="M87" s="5"/>
       <c r="N87" s="17"/>
     </row>
-    <row r="88" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="38"/>
@@ -3232,7 +3267,7 @@
       <c r="M88" s="5"/>
       <c r="N88" s="17"/>
     </row>
-    <row r="89" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="38"/>
@@ -3247,7 +3282,7 @@
       <c r="M89" s="5"/>
       <c r="N89" s="17"/>
     </row>
-    <row r="90" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="38"/>
@@ -3262,7 +3297,7 @@
       <c r="M90" s="5"/>
       <c r="N90" s="17"/>
     </row>
-    <row r="91" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="38"/>
@@ -3277,7 +3312,7 @@
       <c r="M91" s="5"/>
       <c r="N91" s="17"/>
     </row>
-    <row r="92" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="38"/>
@@ -3292,7 +3327,7 @@
       <c r="M92" s="5"/>
       <c r="N92" s="17"/>
     </row>
-    <row r="93" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="38"/>
@@ -3307,7 +3342,7 @@
       <c r="M93" s="5"/>
       <c r="N93" s="17"/>
     </row>
-    <row r="94" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="38"/>
@@ -3322,7 +3357,7 @@
       <c r="M94" s="5"/>
       <c r="N94" s="17"/>
     </row>
-    <row r="95" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="38"/>
@@ -3337,7 +3372,7 @@
       <c r="M95" s="5"/>
       <c r="N95" s="17"/>
     </row>
-    <row r="96" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="38"/>
@@ -3352,7 +3387,7 @@
       <c r="M96" s="5"/>
       <c r="N96" s="17"/>
     </row>
-    <row r="97" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="38"/>
@@ -3367,7 +3402,7 @@
       <c r="M97" s="5"/>
       <c r="N97" s="17"/>
     </row>
-    <row r="98" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="38"/>
@@ -3382,7 +3417,7 @@
       <c r="M98" s="5"/>
       <c r="N98" s="17"/>
     </row>
-    <row r="99" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="38"/>
@@ -3397,7 +3432,7 @@
       <c r="M99" s="5"/>
       <c r="N99" s="17"/>
     </row>
-    <row r="100" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="38"/>
@@ -3412,7 +3447,7 @@
       <c r="M100" s="5"/>
       <c r="N100" s="17"/>
     </row>
-    <row r="101" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="38"/>
@@ -3427,7 +3462,7 @@
       <c r="M101" s="5"/>
       <c r="N101" s="17"/>
     </row>
-    <row r="102" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="38"/>
@@ -3442,7 +3477,7 @@
       <c r="M102" s="5"/>
       <c r="N102" s="17"/>
     </row>
-    <row r="103" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="38"/>
@@ -3457,7 +3492,7 @@
       <c r="M103" s="5"/>
       <c r="N103" s="17"/>
     </row>
-    <row r="104" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="38"/>
@@ -3472,7 +3507,7 @@
       <c r="M104" s="5"/>
       <c r="N104" s="17"/>
     </row>
-    <row r="105" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="38"/>
@@ -3487,7 +3522,7 @@
       <c r="M105" s="5"/>
       <c r="N105" s="17"/>
     </row>
-    <row r="106" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="38"/>
@@ -3502,7 +3537,7 @@
       <c r="M106" s="5"/>
       <c r="N106" s="17"/>
     </row>
-    <row r="107" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="38"/>
@@ -3517,7 +3552,7 @@
       <c r="M107" s="5"/>
       <c r="N107" s="17"/>
     </row>
-    <row r="108" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="38"/>
@@ -3532,7 +3567,7 @@
       <c r="M108" s="5"/>
       <c r="N108" s="17"/>
     </row>
-    <row r="109" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="38"/>
@@ -3547,7 +3582,7 @@
       <c r="M109" s="5"/>
       <c r="N109" s="17"/>
     </row>
-    <row r="110" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="38"/>
@@ -3562,7 +3597,7 @@
       <c r="M110" s="5"/>
       <c r="N110" s="17"/>
     </row>
-    <row r="111" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="38"/>
@@ -3577,7 +3612,7 @@
       <c r="M111" s="5"/>
       <c r="N111" s="17"/>
     </row>
-    <row r="112" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="38"/>
@@ -3592,7 +3627,7 @@
       <c r="M112" s="5"/>
       <c r="N112" s="17"/>
     </row>
-    <row r="113" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="38"/>
@@ -3607,7 +3642,7 @@
       <c r="M113" s="5"/>
       <c r="N113" s="17"/>
     </row>
-    <row r="114" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="38"/>
@@ -3622,7 +3657,7 @@
       <c r="M114" s="5"/>
       <c r="N114" s="17"/>
     </row>
-    <row r="115" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="38"/>
@@ -3637,7 +3672,7 @@
       <c r="M115" s="5"/>
       <c r="N115" s="17"/>
     </row>
-    <row r="116" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="38"/>
@@ -3652,7 +3687,7 @@
       <c r="M116" s="5"/>
       <c r="N116" s="17"/>
     </row>
-    <row r="117" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="38"/>
@@ -3667,7 +3702,7 @@
       <c r="M117" s="5"/>
       <c r="N117" s="17"/>
     </row>
-    <row r="118" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="38"/>
@@ -3682,7 +3717,7 @@
       <c r="M118" s="5"/>
       <c r="N118" s="17"/>
     </row>
-    <row r="119" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="38"/>
@@ -3697,7 +3732,7 @@
       <c r="M119" s="5"/>
       <c r="N119" s="17"/>
     </row>
-    <row r="120" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="38"/>
@@ -3712,7 +3747,7 @@
       <c r="M120" s="5"/>
       <c r="N120" s="17"/>
     </row>
-    <row r="121" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="38"/>
@@ -3727,7 +3762,7 @@
       <c r="M121" s="5"/>
       <c r="N121" s="17"/>
     </row>
-    <row r="122" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="38"/>
@@ -3742,7 +3777,7 @@
       <c r="M122" s="5"/>
       <c r="N122" s="17"/>
     </row>
-    <row r="123" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="123" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="38"/>
@@ -3757,7 +3792,7 @@
       <c r="M123" s="5"/>
       <c r="N123" s="17"/>
     </row>
-    <row r="124" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="124" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="38"/>
@@ -3772,7 +3807,7 @@
       <c r="M124" s="5"/>
       <c r="N124" s="17"/>
     </row>
-    <row r="125" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="125" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="38"/>
@@ -3787,7 +3822,7 @@
       <c r="M125" s="5"/>
       <c r="N125" s="17"/>
     </row>
-    <row r="126" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="126" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="38"/>
@@ -3802,7 +3837,7 @@
       <c r="M126" s="5"/>
       <c r="N126" s="17"/>
     </row>
-    <row r="127" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="127" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="38"/>
@@ -3817,7 +3852,7 @@
       <c r="M127" s="5"/>
       <c r="N127" s="17"/>
     </row>
-    <row r="128" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="128" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="38"/>
@@ -3832,7 +3867,7 @@
       <c r="M128" s="5"/>
       <c r="N128" s="17"/>
     </row>
-    <row r="129" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="129" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="38"/>
@@ -3847,7 +3882,7 @@
       <c r="M129" s="5"/>
       <c r="N129" s="17"/>
     </row>
-    <row r="130" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="130" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="38"/>
@@ -3862,7 +3897,7 @@
       <c r="M130" s="5"/>
       <c r="N130" s="17"/>
     </row>
-    <row r="131" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="131" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="38"/>
@@ -3877,7 +3912,7 @@
       <c r="M131" s="5"/>
       <c r="N131" s="17"/>
     </row>
-    <row r="132" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="38"/>
@@ -3892,7 +3927,7 @@
       <c r="M132" s="5"/>
       <c r="N132" s="17"/>
     </row>
-    <row r="133" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="133" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="38"/>
@@ -3907,7 +3942,7 @@
       <c r="M133" s="5"/>
       <c r="N133" s="17"/>
     </row>
-    <row r="134" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="134" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="38"/>
@@ -3922,7 +3957,7 @@
       <c r="M134" s="5"/>
       <c r="N134" s="17"/>
     </row>
-    <row r="135" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="135" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="38"/>
@@ -3937,7 +3972,7 @@
       <c r="M135" s="5"/>
       <c r="N135" s="17"/>
     </row>
-    <row r="136" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="136" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="38"/>
@@ -3952,7 +3987,7 @@
       <c r="M136" s="5"/>
       <c r="N136" s="17"/>
     </row>
-    <row r="137" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="137" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="38"/>
@@ -3967,7 +4002,7 @@
       <c r="M137" s="5"/>
       <c r="N137" s="17"/>
     </row>
-    <row r="138" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="138" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="38"/>
@@ -3982,7 +4017,7 @@
       <c r="M138" s="5"/>
       <c r="N138" s="17"/>
     </row>
-    <row r="139" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="139" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="38"/>
@@ -3997,7 +4032,7 @@
       <c r="M139" s="5"/>
       <c r="N139" s="17"/>
     </row>
-    <row r="140" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="140" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="38"/>
@@ -4012,7 +4047,7 @@
       <c r="M140" s="5"/>
       <c r="N140" s="17"/>
     </row>
-    <row r="141" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="141" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="38"/>
@@ -4027,7 +4062,7 @@
       <c r="M141" s="5"/>
       <c r="N141" s="17"/>
     </row>
-    <row r="142" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="142" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="38"/>
@@ -4042,7 +4077,7 @@
       <c r="M142" s="5"/>
       <c r="N142" s="17"/>
     </row>
-    <row r="143" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="38"/>
@@ -4057,7 +4092,7 @@
       <c r="M143" s="5"/>
       <c r="N143" s="17"/>
     </row>
-    <row r="144" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="38"/>
@@ -4072,7 +4107,7 @@
       <c r="M144" s="5"/>
       <c r="N144" s="17"/>
     </row>
-    <row r="145" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="145" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="38"/>
@@ -4087,7 +4122,7 @@
       <c r="M145" s="5"/>
       <c r="N145" s="17"/>
     </row>
-    <row r="146" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="146" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="38"/>
@@ -4102,7 +4137,7 @@
       <c r="M146" s="5"/>
       <c r="N146" s="17"/>
     </row>
-    <row r="147" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="147" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="38"/>
@@ -4117,7 +4152,7 @@
       <c r="M147" s="5"/>
       <c r="N147" s="17"/>
     </row>
-    <row r="148" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="148" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="38"/>
@@ -4132,7 +4167,7 @@
       <c r="M148" s="5"/>
       <c r="N148" s="17"/>
     </row>
-    <row r="149" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="149" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="38"/>
@@ -4147,7 +4182,7 @@
       <c r="M149" s="5"/>
       <c r="N149" s="17"/>
     </row>
-    <row r="150" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="150" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="38"/>
@@ -4162,7 +4197,7 @@
       <c r="M150" s="5"/>
       <c r="N150" s="17"/>
     </row>
-    <row r="151" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="151" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="38"/>
@@ -4177,7 +4212,7 @@
       <c r="M151" s="5"/>
       <c r="N151" s="17"/>
     </row>
-    <row r="152" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="152" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="38"/>
@@ -4192,154 +4227,25 @@
       <c r="M152" s="5"/>
       <c r="N152" s="17"/>
     </row>
-    <row r="153" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="153" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="20"/>
       <c r="C153" s="18"/>
-      <c r="D153" s="47"/>
-      <c r="E153" s="48"/>
-      <c r="F153" s="48"/>
-      <c r="G153" s="48"/>
-      <c r="H153" s="48"/>
-      <c r="I153" s="48"/>
-      <c r="J153" s="48"/>
-      <c r="K153" s="49"/>
+      <c r="D153" s="41"/>
+      <c r="E153" s="42"/>
+      <c r="F153" s="42"/>
+      <c r="G153" s="42"/>
+      <c r="H153" s="42"/>
+      <c r="I153" s="42"/>
+      <c r="J153" s="42"/>
+      <c r="K153" s="43"/>
       <c r="L153" s="18"/>
       <c r="M153" s="6"/>
       <c r="N153" s="19"/>
     </row>
-    <row r="154" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="154" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="C7" xr:uid="{6C0B39F1-AC0F-4876-8C89-BECC8B704A99}"/>
   <mergeCells count="147">
-    <mergeCell ref="D152:K152"/>
-    <mergeCell ref="D153:K153"/>
-    <mergeCell ref="D147:K147"/>
-    <mergeCell ref="D148:K148"/>
-    <mergeCell ref="D149:K149"/>
-    <mergeCell ref="D150:K150"/>
-    <mergeCell ref="D151:K151"/>
-    <mergeCell ref="D142:K142"/>
-    <mergeCell ref="D143:K143"/>
-    <mergeCell ref="D144:K144"/>
-    <mergeCell ref="D145:K145"/>
-    <mergeCell ref="D146:K146"/>
-    <mergeCell ref="D137:K137"/>
-    <mergeCell ref="D138:K138"/>
-    <mergeCell ref="D139:K139"/>
-    <mergeCell ref="D140:K140"/>
-    <mergeCell ref="D141:K141"/>
-    <mergeCell ref="D132:K132"/>
-    <mergeCell ref="D133:K133"/>
-    <mergeCell ref="D134:K134"/>
-    <mergeCell ref="D135:K135"/>
-    <mergeCell ref="D136:K136"/>
-    <mergeCell ref="D127:K127"/>
-    <mergeCell ref="D128:K128"/>
-    <mergeCell ref="D129:K129"/>
-    <mergeCell ref="D130:K130"/>
-    <mergeCell ref="D131:K131"/>
-    <mergeCell ref="D122:K122"/>
-    <mergeCell ref="D123:K123"/>
-    <mergeCell ref="D124:K124"/>
-    <mergeCell ref="D125:K125"/>
-    <mergeCell ref="D126:K126"/>
-    <mergeCell ref="D117:K117"/>
-    <mergeCell ref="D118:K118"/>
-    <mergeCell ref="D119:K119"/>
-    <mergeCell ref="D120:K120"/>
-    <mergeCell ref="D121:K121"/>
-    <mergeCell ref="D112:K112"/>
-    <mergeCell ref="D113:K113"/>
-    <mergeCell ref="D114:K114"/>
-    <mergeCell ref="D115:K115"/>
-    <mergeCell ref="D116:K116"/>
-    <mergeCell ref="D107:K107"/>
-    <mergeCell ref="D108:K108"/>
-    <mergeCell ref="D109:K109"/>
-    <mergeCell ref="D110:K110"/>
-    <mergeCell ref="D111:K111"/>
-    <mergeCell ref="D102:K102"/>
-    <mergeCell ref="D103:K103"/>
-    <mergeCell ref="D104:K104"/>
-    <mergeCell ref="D105:K105"/>
-    <mergeCell ref="D106:K106"/>
-    <mergeCell ref="D97:K97"/>
-    <mergeCell ref="D98:K98"/>
-    <mergeCell ref="D99:K99"/>
-    <mergeCell ref="D100:K100"/>
-    <mergeCell ref="D101:K101"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D87:K87"/>
-    <mergeCell ref="D88:K88"/>
-    <mergeCell ref="D89:K89"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D82:K82"/>
-    <mergeCell ref="D83:K83"/>
-    <mergeCell ref="D84:K84"/>
-    <mergeCell ref="D85:K85"/>
-    <mergeCell ref="D86:K86"/>
-    <mergeCell ref="D77:K77"/>
-    <mergeCell ref="D78:K78"/>
-    <mergeCell ref="D79:K79"/>
-    <mergeCell ref="D80:K80"/>
-    <mergeCell ref="D81:K81"/>
-    <mergeCell ref="D72:K72"/>
-    <mergeCell ref="D73:K73"/>
-    <mergeCell ref="D74:K74"/>
-    <mergeCell ref="D75:K75"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D67:K67"/>
-    <mergeCell ref="D68:K68"/>
-    <mergeCell ref="D69:K69"/>
-    <mergeCell ref="D70:K70"/>
-    <mergeCell ref="D71:K71"/>
-    <mergeCell ref="D62:K62"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:K64"/>
-    <mergeCell ref="D65:K65"/>
-    <mergeCell ref="D66:K66"/>
-    <mergeCell ref="D57:K57"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:K59"/>
-    <mergeCell ref="D60:K60"/>
-    <mergeCell ref="D61:K61"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="D54:K54"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="D48:K48"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="D43:K43"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="D32:K32"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="D35:K35"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
@@ -4358,6 +4264,135 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D23:K23"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="D31:K31"/>
+    <mergeCell ref="D32:K32"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="D34:K34"/>
+    <mergeCell ref="D35:K35"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="D48:K48"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="D45:K45"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="D57:K57"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:K59"/>
+    <mergeCell ref="D60:K60"/>
+    <mergeCell ref="D61:K61"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="D54:K54"/>
+    <mergeCell ref="D55:K55"/>
+    <mergeCell ref="D56:K56"/>
+    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="D68:K68"/>
+    <mergeCell ref="D69:K69"/>
+    <mergeCell ref="D70:K70"/>
+    <mergeCell ref="D71:K71"/>
+    <mergeCell ref="D62:K62"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:K64"/>
+    <mergeCell ref="D65:K65"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D72:K72"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="D74:K74"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D87:K87"/>
+    <mergeCell ref="D88:K88"/>
+    <mergeCell ref="D89:K89"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D82:K82"/>
+    <mergeCell ref="D83:K83"/>
+    <mergeCell ref="D84:K84"/>
+    <mergeCell ref="D85:K85"/>
+    <mergeCell ref="D86:K86"/>
+    <mergeCell ref="D97:K97"/>
+    <mergeCell ref="D98:K98"/>
+    <mergeCell ref="D99:K99"/>
+    <mergeCell ref="D100:K100"/>
+    <mergeCell ref="D101:K101"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D107:K107"/>
+    <mergeCell ref="D108:K108"/>
+    <mergeCell ref="D109:K109"/>
+    <mergeCell ref="D110:K110"/>
+    <mergeCell ref="D111:K111"/>
+    <mergeCell ref="D102:K102"/>
+    <mergeCell ref="D103:K103"/>
+    <mergeCell ref="D104:K104"/>
+    <mergeCell ref="D105:K105"/>
+    <mergeCell ref="D106:K106"/>
+    <mergeCell ref="D117:K117"/>
+    <mergeCell ref="D118:K118"/>
+    <mergeCell ref="D119:K119"/>
+    <mergeCell ref="D120:K120"/>
+    <mergeCell ref="D121:K121"/>
+    <mergeCell ref="D112:K112"/>
+    <mergeCell ref="D113:K113"/>
+    <mergeCell ref="D114:K114"/>
+    <mergeCell ref="D115:K115"/>
+    <mergeCell ref="D116:K116"/>
+    <mergeCell ref="D127:K127"/>
+    <mergeCell ref="D128:K128"/>
+    <mergeCell ref="D129:K129"/>
+    <mergeCell ref="D130:K130"/>
+    <mergeCell ref="D131:K131"/>
+    <mergeCell ref="D122:K122"/>
+    <mergeCell ref="D123:K123"/>
+    <mergeCell ref="D124:K124"/>
+    <mergeCell ref="D125:K125"/>
+    <mergeCell ref="D126:K126"/>
+    <mergeCell ref="D137:K137"/>
+    <mergeCell ref="D138:K138"/>
+    <mergeCell ref="D139:K139"/>
+    <mergeCell ref="D140:K140"/>
+    <mergeCell ref="D141:K141"/>
+    <mergeCell ref="D132:K132"/>
+    <mergeCell ref="D133:K133"/>
+    <mergeCell ref="D134:K134"/>
+    <mergeCell ref="D135:K135"/>
+    <mergeCell ref="D136:K136"/>
+    <mergeCell ref="D152:K152"/>
+    <mergeCell ref="D153:K153"/>
+    <mergeCell ref="D147:K147"/>
+    <mergeCell ref="D148:K148"/>
+    <mergeCell ref="D149:K149"/>
+    <mergeCell ref="D150:K150"/>
+    <mergeCell ref="D151:K151"/>
+    <mergeCell ref="D142:K142"/>
+    <mergeCell ref="D143:K143"/>
+    <mergeCell ref="D144:K144"/>
+    <mergeCell ref="D145:K145"/>
+    <mergeCell ref="D146:K146"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C153" xr:uid="{1F00872D-AE43-4317-8957-7AD9F526CA78}">
@@ -4377,159 +4412,153 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57" t="s">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57" t="s">
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="58"/>
-    </row>
-    <row r="3" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58"/>
-    </row>
-    <row r="4" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57" t="s">
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="58"/>
-    </row>
-    <row r="5" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="56"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="58"/>
-    </row>
-    <row r="6" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="58"/>
-    </row>
-    <row r="7" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="58"/>
-    </row>
-    <row r="8" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="50" t="s">
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
+    </row>
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
+    </row>
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
+    </row>
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-    </row>
-    <row r="9" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="55"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="55"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:K3"/>
-    <mergeCell ref="L2:O3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="L4:O5"/>
     <mergeCell ref="D8:O9"/>
     <mergeCell ref="B8:C9"/>
     <mergeCell ref="D4:G5"/>
@@ -4538,6 +4567,12 @@
     <mergeCell ref="H6:K7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="L6:O7"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:K3"/>
+    <mergeCell ref="L2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="L4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adicação de funcionalidades em MQTT, codificação de protobuf, começo de relatorio, etc
</commit_message>
<xml_diff>
--- a/Resource/Tarefas da Semana.xlsx
+++ b/Resource/Tarefas da Semana.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\S.T.A.R\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FE68EB-E5EA-42AA-9DEF-89FA93F2B0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC5A22-2950-46D4-9C6F-F4D8FFC12DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>DATA</t>
   </si>
@@ -148,6 +148,12 @@
   <si>
     <t>Continuação da adição de novas features no projeto, começo do Protobuf, compra de material para o veiculo</t>
   </si>
+  <si>
+    <t>Adição de Features no Launcher</t>
+  </si>
+  <si>
+    <t>Criação de varios tipos de ficheiros e Protobuff efectuado com sucesso</t>
+  </si>
 </sst>
 </file>
 
@@ -942,6 +948,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -951,12 +984,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -966,27 +993,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -996,6 +1002,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1005,22 +1029,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1030,24 +1054,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1333,7 +1339,7 @@
   <dimension ref="A1:XFD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,37 +1351,37 @@
   <sheetData>
     <row r="1" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9 16383:16384" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="36"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="str">
+      <c r="B3" s="30" t="str">
         <f>TEXT(XFC3, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD3, "DD/MM/YYYY")</f>
         <v>03/02/2025 até 09/02/2025</v>
       </c>
       <c r="C3" s="22"/>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
       <c r="XFC3" s="2">
         <v>45691</v>
       </c>
@@ -1384,11 +1390,11 @@
       </c>
     </row>
     <row r="4" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="str">
+      <c r="B4" s="31" t="str">
         <f t="shared" ref="B4:B23" si="0">TEXT(XFC4, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD4, "DD/MM/YYYY")</f>
         <v>10/02/2025 até 16/02/2025</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1406,7 @@
       <c r="H4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="32"/>
       <c r="XFC4" s="2">
         <v>45698</v>
       </c>
@@ -1409,11 +1415,11 @@
       </c>
     </row>
     <row r="5" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="str">
+      <c r="B5" s="31" t="str">
         <f t="shared" si="0"/>
         <v>17/02/2025 até 23/02/2025</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
@@ -1425,7 +1431,7 @@
       <c r="H5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="32"/>
       <c r="XFC5" s="2">
         <v>45705</v>
       </c>
@@ -1434,23 +1440,23 @@
       </c>
     </row>
     <row r="6" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="str">
+      <c r="B6" s="31" t="str">
         <f t="shared" si="0"/>
         <v>24/02/2025 até 02/03/2025</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="22"/>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="32"/>
       <c r="XFC6" s="2">
         <v>45712</v>
       </c>
@@ -1459,11 +1465,11 @@
       </c>
     </row>
     <row r="7" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="str">
+      <c r="B7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>03/03/2025 até 09/03/2025</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="22" t="s">
         <v>31</v>
       </c>
@@ -1471,7 +1477,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
+      <c r="I7" s="32"/>
       <c r="XFC7" s="2">
         <v>45719</v>
       </c>
@@ -1480,19 +1486,19 @@
       </c>
     </row>
     <row r="8" spans="2:9 16383:16384" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="str">
+      <c r="B8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>10/03/2025 até 16/03/2025</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
+      <c r="I8" s="32"/>
       <c r="XFC8" s="2">
         <v>45726</v>
       </c>
@@ -1501,11 +1507,11 @@
       </c>
     </row>
     <row r="9" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="str">
+      <c r="B9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>17/03/2025 até 23/03/2025</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="22" t="s">
         <v>30</v>
       </c>
@@ -1513,7 +1519,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
+      <c r="I9" s="32"/>
       <c r="XFC9" s="2">
         <v>45733</v>
       </c>
@@ -1522,11 +1528,11 @@
       </c>
     </row>
     <row r="10" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="str">
+      <c r="B10" s="31" t="str">
         <f t="shared" si="0"/>
         <v>24/03/2025 até 30/03/2025</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="22" t="s">
         <v>32</v>
       </c>
@@ -1534,7 +1540,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
+      <c r="I10" s="32"/>
       <c r="XFC10" s="2">
         <v>45740</v>
       </c>
@@ -1543,11 +1549,11 @@
       </c>
     </row>
     <row r="11" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="str">
+      <c r="B11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>31/03/2025 até 06/04/2025</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="22" t="s">
         <v>33</v>
       </c>
@@ -1555,7 +1561,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
+      <c r="I11" s="32"/>
       <c r="XFC11" s="2">
         <v>45747</v>
       </c>
@@ -1564,11 +1570,11 @@
       </c>
     </row>
     <row r="12" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="str">
+      <c r="B12" s="31" t="str">
         <f t="shared" si="0"/>
         <v>07/04/2025 até 13/04/2025</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="22" t="s">
         <v>34</v>
       </c>
@@ -1576,7 +1582,7 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
+      <c r="I12" s="32"/>
       <c r="XFC12" s="2">
         <v>45754</v>
       </c>
@@ -1585,11 +1591,11 @@
       </c>
     </row>
     <row r="13" spans="2:9 16383:16384" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="str">
+      <c r="B13" s="31" t="str">
         <f t="shared" si="0"/>
         <v>14/04/2025 até 20/04/2025</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="22" t="s">
         <v>35</v>
       </c>
@@ -1597,7 +1603,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
+      <c r="I13" s="32"/>
       <c r="XFC13" s="2">
         <v>45761</v>
       </c>
@@ -1606,17 +1612,19 @@
       </c>
     </row>
     <row r="14" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="str">
+      <c r="B14" s="31" t="str">
         <f t="shared" si="0"/>
         <v>21/04/2025 até 27/04/2025</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
+      <c r="I14" s="32"/>
       <c r="XFC14" s="2">
         <v>45768</v>
       </c>
@@ -1624,18 +1632,20 @@
         <v>45774</v>
       </c>
     </row>
-    <row r="15" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="26" t="str">
+    <row r="15" spans="2:9 16383:16384" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="31" t="str">
         <f t="shared" si="0"/>
         <v>28/04/2025 até 04/05/2025</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
+      <c r="I15" s="32"/>
       <c r="XFC15" s="2">
         <v>45775</v>
       </c>
@@ -1644,17 +1654,17 @@
       </c>
     </row>
     <row r="16" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="str">
+      <c r="B16" s="31" t="str">
         <f t="shared" si="0"/>
         <v>05/05/2025 até 11/05/2025</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="32"/>
       <c r="XFC16" s="2">
         <v>45782</v>
       </c>
@@ -1663,17 +1673,17 @@
       </c>
     </row>
     <row r="17" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="26" t="str">
+      <c r="B17" s="31" t="str">
         <f t="shared" si="0"/>
         <v>12/05/2025 até 18/05/2025</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="32"/>
       <c r="XFC17" s="2">
         <v>45789</v>
       </c>
@@ -1682,17 +1692,17 @@
       </c>
     </row>
     <row r="18" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="str">
+      <c r="B18" s="31" t="str">
         <f t="shared" si="0"/>
         <v>19/05/2025 até 25/05/2025</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
+      <c r="I18" s="32"/>
       <c r="XFC18" s="2">
         <v>45796</v>
       </c>
@@ -1701,17 +1711,17 @@
       </c>
     </row>
     <row r="19" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="str">
+      <c r="B19" s="31" t="str">
         <f t="shared" si="0"/>
         <v>26/05/2025 até 01/06/2025</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
+      <c r="I19" s="32"/>
       <c r="XFC19" s="2">
         <v>45803</v>
       </c>
@@ -1720,17 +1730,17 @@
       </c>
     </row>
     <row r="20" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="str">
+      <c r="B20" s="31" t="str">
         <f t="shared" si="0"/>
         <v>02/06/2025 até 08/06/2025</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="32"/>
       <c r="XFC20" s="2">
         <v>45810</v>
       </c>
@@ -1739,17 +1749,17 @@
       </c>
     </row>
     <row r="21" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="str">
+      <c r="B21" s="31" t="str">
         <f t="shared" si="0"/>
         <v>09/06/2025 até 15/06/2025</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="32"/>
       <c r="XFC21" s="2">
         <v>45817</v>
       </c>
@@ -1758,17 +1768,17 @@
       </c>
     </row>
     <row r="22" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="31" t="str">
         <f t="shared" si="0"/>
         <v>16/06/2025 até 22/06/2025</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="32"/>
       <c r="XFC22" s="2">
         <v>45824</v>
       </c>
@@ -1777,17 +1787,17 @@
       </c>
     </row>
     <row r="23" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="str">
+      <c r="B23" s="31" t="str">
         <f t="shared" si="0"/>
         <v>23/06/2025 até 29/06/2025</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
+      <c r="I23" s="32"/>
       <c r="XFC23" s="2">
         <v>45831</v>
       </c>
@@ -1796,17 +1806,17 @@
       </c>
     </row>
     <row r="24" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="str">
+      <c r="B24" s="31" t="str">
         <f t="shared" ref="B24:B25" si="1">TEXT(XFC24, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD24, "DD/MM/YYYY")</f>
         <v>30/06/2025 até 06/07/2025</v>
       </c>
-      <c r="C24" s="27"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
+      <c r="I24" s="32"/>
       <c r="XFC24" s="2">
         <v>45838</v>
       </c>
@@ -1815,17 +1825,17 @@
       </c>
     </row>
     <row r="25" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="str">
+      <c r="B25" s="35" t="str">
         <f t="shared" si="1"/>
         <v>07/07/2025 até 13/07/2025</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="30"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="37"/>
       <c r="XFC25" s="2">
         <v>45845</v>
       </c>
@@ -1834,28 +1844,79 @@
       </c>
     </row>
     <row r="26" spans="2:9 16383:16384" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
     </row>
     <row r="27" spans="2:9 16383:16384" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="F7:G7"/>
@@ -1872,73 +1933,22 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H23:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1980,16 +1990,16 @@
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
       <c r="L7" s="10" t="s">
         <v>1</v>
       </c>
@@ -2010,16 +2020,16 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="13" t="s">
         <v>13</v>
       </c>
@@ -4230,14 +4240,14 @@
     <row r="153" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="20"/>
       <c r="C153" s="18"/>
-      <c r="D153" s="41"/>
-      <c r="E153" s="42"/>
-      <c r="F153" s="42"/>
-      <c r="G153" s="42"/>
-      <c r="H153" s="42"/>
-      <c r="I153" s="42"/>
-      <c r="J153" s="42"/>
-      <c r="K153" s="43"/>
+      <c r="D153" s="47"/>
+      <c r="E153" s="48"/>
+      <c r="F153" s="48"/>
+      <c r="G153" s="48"/>
+      <c r="H153" s="48"/>
+      <c r="I153" s="48"/>
+      <c r="J153" s="48"/>
+      <c r="K153" s="49"/>
       <c r="L153" s="18"/>
       <c r="M153" s="6"/>
       <c r="N153" s="19"/>
@@ -4246,6 +4256,135 @@
   </sheetData>
   <autoFilter ref="C7" xr:uid="{6C0B39F1-AC0F-4876-8C89-BECC8B704A99}"/>
   <mergeCells count="147">
+    <mergeCell ref="D152:K152"/>
+    <mergeCell ref="D153:K153"/>
+    <mergeCell ref="D147:K147"/>
+    <mergeCell ref="D148:K148"/>
+    <mergeCell ref="D149:K149"/>
+    <mergeCell ref="D150:K150"/>
+    <mergeCell ref="D151:K151"/>
+    <mergeCell ref="D142:K142"/>
+    <mergeCell ref="D143:K143"/>
+    <mergeCell ref="D144:K144"/>
+    <mergeCell ref="D145:K145"/>
+    <mergeCell ref="D146:K146"/>
+    <mergeCell ref="D137:K137"/>
+    <mergeCell ref="D138:K138"/>
+    <mergeCell ref="D139:K139"/>
+    <mergeCell ref="D140:K140"/>
+    <mergeCell ref="D141:K141"/>
+    <mergeCell ref="D132:K132"/>
+    <mergeCell ref="D133:K133"/>
+    <mergeCell ref="D134:K134"/>
+    <mergeCell ref="D135:K135"/>
+    <mergeCell ref="D136:K136"/>
+    <mergeCell ref="D127:K127"/>
+    <mergeCell ref="D128:K128"/>
+    <mergeCell ref="D129:K129"/>
+    <mergeCell ref="D130:K130"/>
+    <mergeCell ref="D131:K131"/>
+    <mergeCell ref="D122:K122"/>
+    <mergeCell ref="D123:K123"/>
+    <mergeCell ref="D124:K124"/>
+    <mergeCell ref="D125:K125"/>
+    <mergeCell ref="D126:K126"/>
+    <mergeCell ref="D117:K117"/>
+    <mergeCell ref="D118:K118"/>
+    <mergeCell ref="D119:K119"/>
+    <mergeCell ref="D120:K120"/>
+    <mergeCell ref="D121:K121"/>
+    <mergeCell ref="D112:K112"/>
+    <mergeCell ref="D113:K113"/>
+    <mergeCell ref="D114:K114"/>
+    <mergeCell ref="D115:K115"/>
+    <mergeCell ref="D116:K116"/>
+    <mergeCell ref="D107:K107"/>
+    <mergeCell ref="D108:K108"/>
+    <mergeCell ref="D109:K109"/>
+    <mergeCell ref="D110:K110"/>
+    <mergeCell ref="D111:K111"/>
+    <mergeCell ref="D102:K102"/>
+    <mergeCell ref="D103:K103"/>
+    <mergeCell ref="D104:K104"/>
+    <mergeCell ref="D105:K105"/>
+    <mergeCell ref="D106:K106"/>
+    <mergeCell ref="D97:K97"/>
+    <mergeCell ref="D98:K98"/>
+    <mergeCell ref="D99:K99"/>
+    <mergeCell ref="D100:K100"/>
+    <mergeCell ref="D101:K101"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D87:K87"/>
+    <mergeCell ref="D88:K88"/>
+    <mergeCell ref="D89:K89"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D82:K82"/>
+    <mergeCell ref="D83:K83"/>
+    <mergeCell ref="D84:K84"/>
+    <mergeCell ref="D85:K85"/>
+    <mergeCell ref="D86:K86"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D72:K72"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="D74:K74"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="D68:K68"/>
+    <mergeCell ref="D69:K69"/>
+    <mergeCell ref="D70:K70"/>
+    <mergeCell ref="D71:K71"/>
+    <mergeCell ref="D62:K62"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:K64"/>
+    <mergeCell ref="D65:K65"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D57:K57"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:K59"/>
+    <mergeCell ref="D60:K60"/>
+    <mergeCell ref="D61:K61"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="D54:K54"/>
+    <mergeCell ref="D55:K55"/>
+    <mergeCell ref="D56:K56"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="D48:K48"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="D45:K45"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="D31:K31"/>
+    <mergeCell ref="D32:K32"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="D34:K34"/>
+    <mergeCell ref="D35:K35"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
@@ -4264,135 +4403,6 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D23:K23"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="D32:K32"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="D35:K35"/>
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="D48:K48"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="D43:K43"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="D57:K57"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:K59"/>
-    <mergeCell ref="D60:K60"/>
-    <mergeCell ref="D61:K61"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="D54:K54"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="D67:K67"/>
-    <mergeCell ref="D68:K68"/>
-    <mergeCell ref="D69:K69"/>
-    <mergeCell ref="D70:K70"/>
-    <mergeCell ref="D71:K71"/>
-    <mergeCell ref="D62:K62"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:K64"/>
-    <mergeCell ref="D65:K65"/>
-    <mergeCell ref="D66:K66"/>
-    <mergeCell ref="D77:K77"/>
-    <mergeCell ref="D78:K78"/>
-    <mergeCell ref="D79:K79"/>
-    <mergeCell ref="D80:K80"/>
-    <mergeCell ref="D81:K81"/>
-    <mergeCell ref="D72:K72"/>
-    <mergeCell ref="D73:K73"/>
-    <mergeCell ref="D74:K74"/>
-    <mergeCell ref="D75:K75"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D87:K87"/>
-    <mergeCell ref="D88:K88"/>
-    <mergeCell ref="D89:K89"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D82:K82"/>
-    <mergeCell ref="D83:K83"/>
-    <mergeCell ref="D84:K84"/>
-    <mergeCell ref="D85:K85"/>
-    <mergeCell ref="D86:K86"/>
-    <mergeCell ref="D97:K97"/>
-    <mergeCell ref="D98:K98"/>
-    <mergeCell ref="D99:K99"/>
-    <mergeCell ref="D100:K100"/>
-    <mergeCell ref="D101:K101"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D107:K107"/>
-    <mergeCell ref="D108:K108"/>
-    <mergeCell ref="D109:K109"/>
-    <mergeCell ref="D110:K110"/>
-    <mergeCell ref="D111:K111"/>
-    <mergeCell ref="D102:K102"/>
-    <mergeCell ref="D103:K103"/>
-    <mergeCell ref="D104:K104"/>
-    <mergeCell ref="D105:K105"/>
-    <mergeCell ref="D106:K106"/>
-    <mergeCell ref="D117:K117"/>
-    <mergeCell ref="D118:K118"/>
-    <mergeCell ref="D119:K119"/>
-    <mergeCell ref="D120:K120"/>
-    <mergeCell ref="D121:K121"/>
-    <mergeCell ref="D112:K112"/>
-    <mergeCell ref="D113:K113"/>
-    <mergeCell ref="D114:K114"/>
-    <mergeCell ref="D115:K115"/>
-    <mergeCell ref="D116:K116"/>
-    <mergeCell ref="D127:K127"/>
-    <mergeCell ref="D128:K128"/>
-    <mergeCell ref="D129:K129"/>
-    <mergeCell ref="D130:K130"/>
-    <mergeCell ref="D131:K131"/>
-    <mergeCell ref="D122:K122"/>
-    <mergeCell ref="D123:K123"/>
-    <mergeCell ref="D124:K124"/>
-    <mergeCell ref="D125:K125"/>
-    <mergeCell ref="D126:K126"/>
-    <mergeCell ref="D137:K137"/>
-    <mergeCell ref="D138:K138"/>
-    <mergeCell ref="D139:K139"/>
-    <mergeCell ref="D140:K140"/>
-    <mergeCell ref="D141:K141"/>
-    <mergeCell ref="D132:K132"/>
-    <mergeCell ref="D133:K133"/>
-    <mergeCell ref="D134:K134"/>
-    <mergeCell ref="D135:K135"/>
-    <mergeCell ref="D136:K136"/>
-    <mergeCell ref="D152:K152"/>
-    <mergeCell ref="D153:K153"/>
-    <mergeCell ref="D147:K147"/>
-    <mergeCell ref="D148:K148"/>
-    <mergeCell ref="D149:K149"/>
-    <mergeCell ref="D150:K150"/>
-    <mergeCell ref="D151:K151"/>
-    <mergeCell ref="D142:K142"/>
-    <mergeCell ref="D143:K143"/>
-    <mergeCell ref="D144:K144"/>
-    <mergeCell ref="D145:K145"/>
-    <mergeCell ref="D146:K146"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C153" xr:uid="{1F00872D-AE43-4317-8957-7AD9F526CA78}">
@@ -4416,149 +4426,155 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51" t="s">
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51" t="s">
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="58"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51" t="s">
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="58"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="58"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="53" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="55"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="58"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:K3"/>
+    <mergeCell ref="L2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="L4:O5"/>
     <mergeCell ref="D8:O9"/>
     <mergeCell ref="B8:C9"/>
     <mergeCell ref="D4:G5"/>
@@ -4567,12 +4583,6 @@
     <mergeCell ref="H6:K7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="L6:O7"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:K3"/>
-    <mergeCell ref="L2:O3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="L4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizacao de relatorio e rosa
</commit_message>
<xml_diff>
--- a/Resource/Tarefas da Semana.xlsx
+++ b/Resource/Tarefas da Semana.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\S.T.A.R\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC5A22-2950-46D4-9C6F-F4D8FFC12DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BFF264-5DC6-4B60-AB0A-467861273750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>DATA</t>
   </si>
@@ -154,6 +154,15 @@
   <si>
     <t>Criação de varios tipos de ficheiros e Protobuff efectuado com sucesso</t>
   </si>
+  <si>
+    <t>Começo do projeto e equipamento IOT</t>
+  </si>
+  <si>
+    <t>Ligação do mesmo e reconhecimento do codigo IOT</t>
+  </si>
+  <si>
+    <t>IA a funcionar!</t>
+  </si>
 </sst>
 </file>
 
@@ -948,18 +957,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,27 +1002,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1002,6 +1011,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,14 +1038,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1045,15 +1063,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,7 +1348,7 @@
   <dimension ref="A1:XFD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,37 +1360,37 @@
   <sheetData>
     <row r="1" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9 16383:16384" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="2:9 16383:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="str">
+      <c r="B3" s="37" t="str">
         <f>TEXT(XFC3, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD3, "DD/MM/YYYY")</f>
         <v>03/02/2025 até 09/02/2025</v>
       </c>
       <c r="C3" s="22"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
       <c r="XFC3" s="2">
         <v>45691</v>
       </c>
@@ -1390,11 +1399,11 @@
       </c>
     </row>
     <row r="4" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="str">
+      <c r="B4" s="26" t="str">
         <f t="shared" ref="B4:B23" si="0">TEXT(XFC4, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD4, "DD/MM/YYYY")</f>
         <v>10/02/2025 até 16/02/2025</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1415,7 @@
       <c r="H4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="32"/>
+      <c r="I4" s="23"/>
       <c r="XFC4" s="2">
         <v>45698</v>
       </c>
@@ -1415,11 +1424,11 @@
       </c>
     </row>
     <row r="5" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31" t="str">
+      <c r="B5" s="26" t="str">
         <f t="shared" si="0"/>
         <v>17/02/2025 até 23/02/2025</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
@@ -1431,7 +1440,7 @@
       <c r="H5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="23"/>
       <c r="XFC5" s="2">
         <v>45705</v>
       </c>
@@ -1440,23 +1449,23 @@
       </c>
     </row>
     <row r="6" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="str">
+      <c r="B6" s="26" t="str">
         <f t="shared" si="0"/>
         <v>24/02/2025 até 02/03/2025</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="22"/>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="23"/>
       <c r="XFC6" s="2">
         <v>45712</v>
       </c>
@@ -1465,11 +1474,11 @@
       </c>
     </row>
     <row r="7" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="str">
+      <c r="B7" s="26" t="str">
         <f t="shared" si="0"/>
         <v>03/03/2025 até 09/03/2025</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="22" t="s">
         <v>31</v>
       </c>
@@ -1477,7 +1486,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
-      <c r="I7" s="32"/>
+      <c r="I7" s="23"/>
       <c r="XFC7" s="2">
         <v>45719</v>
       </c>
@@ -1486,19 +1495,19 @@
       </c>
     </row>
     <row r="8" spans="2:9 16383:16384" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="str">
+      <c r="B8" s="26" t="str">
         <f t="shared" si="0"/>
         <v>10/03/2025 até 16/03/2025</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="26"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
-      <c r="I8" s="32"/>
+      <c r="I8" s="23"/>
       <c r="XFC8" s="2">
         <v>45726</v>
       </c>
@@ -1507,11 +1516,11 @@
       </c>
     </row>
     <row r="9" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="str">
+      <c r="B9" s="26" t="str">
         <f t="shared" si="0"/>
         <v>17/03/2025 até 23/03/2025</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="22" t="s">
         <v>30</v>
       </c>
@@ -1519,7 +1528,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="32"/>
+      <c r="I9" s="23"/>
       <c r="XFC9" s="2">
         <v>45733</v>
       </c>
@@ -1528,11 +1537,11 @@
       </c>
     </row>
     <row r="10" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="str">
+      <c r="B10" s="26" t="str">
         <f t="shared" si="0"/>
         <v>24/03/2025 até 30/03/2025</v>
       </c>
-      <c r="C10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="22" t="s">
         <v>32</v>
       </c>
@@ -1540,7 +1549,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
-      <c r="I10" s="32"/>
+      <c r="I10" s="23"/>
       <c r="XFC10" s="2">
         <v>45740</v>
       </c>
@@ -1549,11 +1558,11 @@
       </c>
     </row>
     <row r="11" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="str">
+      <c r="B11" s="26" t="str">
         <f t="shared" si="0"/>
         <v>31/03/2025 até 06/04/2025</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="22" t="s">
         <v>33</v>
       </c>
@@ -1561,7 +1570,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
-      <c r="I11" s="32"/>
+      <c r="I11" s="23"/>
       <c r="XFC11" s="2">
         <v>45747</v>
       </c>
@@ -1570,11 +1579,11 @@
       </c>
     </row>
     <row r="12" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31" t="str">
+      <c r="B12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>07/04/2025 até 13/04/2025</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="22" t="s">
         <v>34</v>
       </c>
@@ -1582,7 +1591,7 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
-      <c r="I12" s="32"/>
+      <c r="I12" s="23"/>
       <c r="XFC12" s="2">
         <v>45754</v>
       </c>
@@ -1591,11 +1600,11 @@
       </c>
     </row>
     <row r="13" spans="2:9 16383:16384" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31" t="str">
+      <c r="B13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>14/04/2025 até 20/04/2025</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="22" t="s">
         <v>35</v>
       </c>
@@ -1603,7 +1612,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
-      <c r="I13" s="32"/>
+      <c r="I13" s="23"/>
       <c r="XFC13" s="2">
         <v>45761</v>
       </c>
@@ -1612,11 +1621,11 @@
       </c>
     </row>
     <row r="14" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="str">
+      <c r="B14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>21/04/2025 até 27/04/2025</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="22" t="s">
         <v>36</v>
       </c>
@@ -1624,7 +1633,7 @@
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
-      <c r="I14" s="32"/>
+      <c r="I14" s="23"/>
       <c r="XFC14" s="2">
         <v>45768</v>
       </c>
@@ -1633,11 +1642,11 @@
       </c>
     </row>
     <row r="15" spans="2:9 16383:16384" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="31" t="str">
+      <c r="B15" s="26" t="str">
         <f t="shared" si="0"/>
         <v>28/04/2025 até 04/05/2025</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="22" t="s">
         <v>37</v>
       </c>
@@ -1645,7 +1654,7 @@
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="32"/>
+      <c r="I15" s="23"/>
       <c r="XFC15" s="2">
         <v>45775</v>
       </c>
@@ -1654,17 +1663,19 @@
       </c>
     </row>
     <row r="16" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31" t="str">
+      <c r="B16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>05/05/2025 até 11/05/2025</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
-      <c r="I16" s="32"/>
+      <c r="I16" s="23"/>
       <c r="XFC16" s="2">
         <v>45782</v>
       </c>
@@ -1673,17 +1684,19 @@
       </c>
     </row>
     <row r="17" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31" t="str">
+      <c r="B17" s="26" t="str">
         <f t="shared" si="0"/>
         <v>12/05/2025 até 18/05/2025</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="23"/>
       <c r="XFC17" s="2">
         <v>45789</v>
       </c>
@@ -1692,17 +1705,19 @@
       </c>
     </row>
     <row r="18" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31" t="str">
+      <c r="B18" s="26" t="str">
         <f t="shared" si="0"/>
         <v>19/05/2025 até 25/05/2025</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="32"/>
+      <c r="I18" s="23"/>
       <c r="XFC18" s="2">
         <v>45796</v>
       </c>
@@ -1711,17 +1726,17 @@
       </c>
     </row>
     <row r="19" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31" t="str">
+      <c r="B19" s="26" t="str">
         <f t="shared" si="0"/>
         <v>26/05/2025 até 01/06/2025</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="23"/>
       <c r="XFC19" s="2">
         <v>45803</v>
       </c>
@@ -1730,17 +1745,17 @@
       </c>
     </row>
     <row r="20" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31" t="str">
+      <c r="B20" s="26" t="str">
         <f t="shared" si="0"/>
         <v>02/06/2025 até 08/06/2025</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="32"/>
+      <c r="I20" s="23"/>
       <c r="XFC20" s="2">
         <v>45810</v>
       </c>
@@ -1749,17 +1764,17 @@
       </c>
     </row>
     <row r="21" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="str">
+      <c r="B21" s="26" t="str">
         <f t="shared" si="0"/>
         <v>09/06/2025 até 15/06/2025</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="23"/>
       <c r="XFC21" s="2">
         <v>45817</v>
       </c>
@@ -1768,17 +1783,17 @@
       </c>
     </row>
     <row r="22" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="str">
+      <c r="B22" s="26" t="str">
         <f t="shared" si="0"/>
         <v>16/06/2025 até 22/06/2025</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="32"/>
+      <c r="I22" s="23"/>
       <c r="XFC22" s="2">
         <v>45824</v>
       </c>
@@ -1787,17 +1802,17 @@
       </c>
     </row>
     <row r="23" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="str">
+      <c r="B23" s="26" t="str">
         <f t="shared" si="0"/>
         <v>23/06/2025 até 29/06/2025</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="23"/>
       <c r="XFC23" s="2">
         <v>45831</v>
       </c>
@@ -1806,17 +1821,17 @@
       </c>
     </row>
     <row r="24" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="31" t="str">
+      <c r="B24" s="26" t="str">
         <f t="shared" ref="B24:B25" si="1">TEXT(XFC24, "DD/MM/YYYY") &amp; " até " &amp; TEXT(XFD24, "DD/MM/YYYY")</f>
         <v>30/06/2025 até 06/07/2025</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="23"/>
       <c r="XFC24" s="2">
         <v>45838</v>
       </c>
@@ -1825,17 +1840,17 @@
       </c>
     </row>
     <row r="25" spans="2:9 16383:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="str">
+      <c r="B25" s="28" t="str">
         <f t="shared" si="1"/>
         <v>07/07/2025 até 13/07/2025</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="37"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="30"/>
       <c r="XFC25" s="2">
         <v>45845</v>
       </c>
@@ -1844,15 +1859,95 @@
       </c>
     </row>
     <row r="26" spans="2:9 16383:16384" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="27" spans="2:9 16383:16384" x14ac:dyDescent="0.25">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D24:E24"/>
@@ -1869,86 +1964,6 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1990,16 +2005,16 @@
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="46"/>
       <c r="L7" s="10" t="s">
         <v>1</v>
       </c>
@@ -2020,16 +2035,16 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="13" t="s">
         <v>13</v>
       </c>
@@ -4240,14 +4255,14 @@
     <row r="153" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="20"/>
       <c r="C153" s="18"/>
-      <c r="D153" s="47"/>
-      <c r="E153" s="48"/>
-      <c r="F153" s="48"/>
-      <c r="G153" s="48"/>
-      <c r="H153" s="48"/>
-      <c r="I153" s="48"/>
-      <c r="J153" s="48"/>
-      <c r="K153" s="49"/>
+      <c r="D153" s="41"/>
+      <c r="E153" s="42"/>
+      <c r="F153" s="42"/>
+      <c r="G153" s="42"/>
+      <c r="H153" s="42"/>
+      <c r="I153" s="42"/>
+      <c r="J153" s="42"/>
+      <c r="K153" s="43"/>
       <c r="L153" s="18"/>
       <c r="M153" s="6"/>
       <c r="N153" s="19"/>
@@ -4256,135 +4271,6 @@
   </sheetData>
   <autoFilter ref="C7" xr:uid="{6C0B39F1-AC0F-4876-8C89-BECC8B704A99}"/>
   <mergeCells count="147">
-    <mergeCell ref="D152:K152"/>
-    <mergeCell ref="D153:K153"/>
-    <mergeCell ref="D147:K147"/>
-    <mergeCell ref="D148:K148"/>
-    <mergeCell ref="D149:K149"/>
-    <mergeCell ref="D150:K150"/>
-    <mergeCell ref="D151:K151"/>
-    <mergeCell ref="D142:K142"/>
-    <mergeCell ref="D143:K143"/>
-    <mergeCell ref="D144:K144"/>
-    <mergeCell ref="D145:K145"/>
-    <mergeCell ref="D146:K146"/>
-    <mergeCell ref="D137:K137"/>
-    <mergeCell ref="D138:K138"/>
-    <mergeCell ref="D139:K139"/>
-    <mergeCell ref="D140:K140"/>
-    <mergeCell ref="D141:K141"/>
-    <mergeCell ref="D132:K132"/>
-    <mergeCell ref="D133:K133"/>
-    <mergeCell ref="D134:K134"/>
-    <mergeCell ref="D135:K135"/>
-    <mergeCell ref="D136:K136"/>
-    <mergeCell ref="D127:K127"/>
-    <mergeCell ref="D128:K128"/>
-    <mergeCell ref="D129:K129"/>
-    <mergeCell ref="D130:K130"/>
-    <mergeCell ref="D131:K131"/>
-    <mergeCell ref="D122:K122"/>
-    <mergeCell ref="D123:K123"/>
-    <mergeCell ref="D124:K124"/>
-    <mergeCell ref="D125:K125"/>
-    <mergeCell ref="D126:K126"/>
-    <mergeCell ref="D117:K117"/>
-    <mergeCell ref="D118:K118"/>
-    <mergeCell ref="D119:K119"/>
-    <mergeCell ref="D120:K120"/>
-    <mergeCell ref="D121:K121"/>
-    <mergeCell ref="D112:K112"/>
-    <mergeCell ref="D113:K113"/>
-    <mergeCell ref="D114:K114"/>
-    <mergeCell ref="D115:K115"/>
-    <mergeCell ref="D116:K116"/>
-    <mergeCell ref="D107:K107"/>
-    <mergeCell ref="D108:K108"/>
-    <mergeCell ref="D109:K109"/>
-    <mergeCell ref="D110:K110"/>
-    <mergeCell ref="D111:K111"/>
-    <mergeCell ref="D102:K102"/>
-    <mergeCell ref="D103:K103"/>
-    <mergeCell ref="D104:K104"/>
-    <mergeCell ref="D105:K105"/>
-    <mergeCell ref="D106:K106"/>
-    <mergeCell ref="D97:K97"/>
-    <mergeCell ref="D98:K98"/>
-    <mergeCell ref="D99:K99"/>
-    <mergeCell ref="D100:K100"/>
-    <mergeCell ref="D101:K101"/>
-    <mergeCell ref="D92:K92"/>
-    <mergeCell ref="D93:K93"/>
-    <mergeCell ref="D94:K94"/>
-    <mergeCell ref="D95:K95"/>
-    <mergeCell ref="D96:K96"/>
-    <mergeCell ref="D87:K87"/>
-    <mergeCell ref="D88:K88"/>
-    <mergeCell ref="D89:K89"/>
-    <mergeCell ref="D90:K90"/>
-    <mergeCell ref="D91:K91"/>
-    <mergeCell ref="D82:K82"/>
-    <mergeCell ref="D83:K83"/>
-    <mergeCell ref="D84:K84"/>
-    <mergeCell ref="D85:K85"/>
-    <mergeCell ref="D86:K86"/>
-    <mergeCell ref="D77:K77"/>
-    <mergeCell ref="D78:K78"/>
-    <mergeCell ref="D79:K79"/>
-    <mergeCell ref="D80:K80"/>
-    <mergeCell ref="D81:K81"/>
-    <mergeCell ref="D72:K72"/>
-    <mergeCell ref="D73:K73"/>
-    <mergeCell ref="D74:K74"/>
-    <mergeCell ref="D75:K75"/>
-    <mergeCell ref="D76:K76"/>
-    <mergeCell ref="D67:K67"/>
-    <mergeCell ref="D68:K68"/>
-    <mergeCell ref="D69:K69"/>
-    <mergeCell ref="D70:K70"/>
-    <mergeCell ref="D71:K71"/>
-    <mergeCell ref="D62:K62"/>
-    <mergeCell ref="D63:K63"/>
-    <mergeCell ref="D64:K64"/>
-    <mergeCell ref="D65:K65"/>
-    <mergeCell ref="D66:K66"/>
-    <mergeCell ref="D57:K57"/>
-    <mergeCell ref="D58:K58"/>
-    <mergeCell ref="D59:K59"/>
-    <mergeCell ref="D60:K60"/>
-    <mergeCell ref="D61:K61"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="D54:K54"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="D48:K48"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="D43:K43"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="D32:K32"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="D35:K35"/>
     <mergeCell ref="D12:K12"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D8:K8"/>
@@ -4403,6 +4289,135 @@
     <mergeCell ref="D21:K21"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D23:K23"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="D31:K31"/>
+    <mergeCell ref="D32:K32"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="D34:K34"/>
+    <mergeCell ref="D35:K35"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="D48:K48"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="D45:K45"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="D57:K57"/>
+    <mergeCell ref="D58:K58"/>
+    <mergeCell ref="D59:K59"/>
+    <mergeCell ref="D60:K60"/>
+    <mergeCell ref="D61:K61"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="D54:K54"/>
+    <mergeCell ref="D55:K55"/>
+    <mergeCell ref="D56:K56"/>
+    <mergeCell ref="D67:K67"/>
+    <mergeCell ref="D68:K68"/>
+    <mergeCell ref="D69:K69"/>
+    <mergeCell ref="D70:K70"/>
+    <mergeCell ref="D71:K71"/>
+    <mergeCell ref="D62:K62"/>
+    <mergeCell ref="D63:K63"/>
+    <mergeCell ref="D64:K64"/>
+    <mergeCell ref="D65:K65"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D77:K77"/>
+    <mergeCell ref="D78:K78"/>
+    <mergeCell ref="D79:K79"/>
+    <mergeCell ref="D80:K80"/>
+    <mergeCell ref="D81:K81"/>
+    <mergeCell ref="D72:K72"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="D74:K74"/>
+    <mergeCell ref="D75:K75"/>
+    <mergeCell ref="D76:K76"/>
+    <mergeCell ref="D87:K87"/>
+    <mergeCell ref="D88:K88"/>
+    <mergeCell ref="D89:K89"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D82:K82"/>
+    <mergeCell ref="D83:K83"/>
+    <mergeCell ref="D84:K84"/>
+    <mergeCell ref="D85:K85"/>
+    <mergeCell ref="D86:K86"/>
+    <mergeCell ref="D97:K97"/>
+    <mergeCell ref="D98:K98"/>
+    <mergeCell ref="D99:K99"/>
+    <mergeCell ref="D100:K100"/>
+    <mergeCell ref="D101:K101"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D107:K107"/>
+    <mergeCell ref="D108:K108"/>
+    <mergeCell ref="D109:K109"/>
+    <mergeCell ref="D110:K110"/>
+    <mergeCell ref="D111:K111"/>
+    <mergeCell ref="D102:K102"/>
+    <mergeCell ref="D103:K103"/>
+    <mergeCell ref="D104:K104"/>
+    <mergeCell ref="D105:K105"/>
+    <mergeCell ref="D106:K106"/>
+    <mergeCell ref="D117:K117"/>
+    <mergeCell ref="D118:K118"/>
+    <mergeCell ref="D119:K119"/>
+    <mergeCell ref="D120:K120"/>
+    <mergeCell ref="D121:K121"/>
+    <mergeCell ref="D112:K112"/>
+    <mergeCell ref="D113:K113"/>
+    <mergeCell ref="D114:K114"/>
+    <mergeCell ref="D115:K115"/>
+    <mergeCell ref="D116:K116"/>
+    <mergeCell ref="D127:K127"/>
+    <mergeCell ref="D128:K128"/>
+    <mergeCell ref="D129:K129"/>
+    <mergeCell ref="D130:K130"/>
+    <mergeCell ref="D131:K131"/>
+    <mergeCell ref="D122:K122"/>
+    <mergeCell ref="D123:K123"/>
+    <mergeCell ref="D124:K124"/>
+    <mergeCell ref="D125:K125"/>
+    <mergeCell ref="D126:K126"/>
+    <mergeCell ref="D137:K137"/>
+    <mergeCell ref="D138:K138"/>
+    <mergeCell ref="D139:K139"/>
+    <mergeCell ref="D140:K140"/>
+    <mergeCell ref="D141:K141"/>
+    <mergeCell ref="D132:K132"/>
+    <mergeCell ref="D133:K133"/>
+    <mergeCell ref="D134:K134"/>
+    <mergeCell ref="D135:K135"/>
+    <mergeCell ref="D136:K136"/>
+    <mergeCell ref="D152:K152"/>
+    <mergeCell ref="D153:K153"/>
+    <mergeCell ref="D147:K147"/>
+    <mergeCell ref="D148:K148"/>
+    <mergeCell ref="D149:K149"/>
+    <mergeCell ref="D150:K150"/>
+    <mergeCell ref="D151:K151"/>
+    <mergeCell ref="D142:K142"/>
+    <mergeCell ref="D143:K143"/>
+    <mergeCell ref="D144:K144"/>
+    <mergeCell ref="D145:K145"/>
+    <mergeCell ref="D146:K146"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C153" xr:uid="{1F00872D-AE43-4317-8957-7AD9F526CA78}">
@@ -4426,155 +4441,149 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57" t="s">
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="58"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57" t="s">
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="58"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="56"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="58"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="58"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="58"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="52"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="50" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="55"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="55"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:K3"/>
-    <mergeCell ref="L2:O3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="L4:O5"/>
     <mergeCell ref="D8:O9"/>
     <mergeCell ref="B8:C9"/>
     <mergeCell ref="D4:G5"/>
@@ -4583,6 +4592,12 @@
     <mergeCell ref="H6:K7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="L6:O7"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:K3"/>
+    <mergeCell ref="L2:O3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="L4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>